<commit_message>
Đổi tên model User -> Member (tên User bị lỗi), Chỉnh lại giao diện bài đào tạo + thêm chức năng tìm kiếm với LabID của BNS
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/training.xlsx
+++ b/Hethongquanlylab/wwwroot/data/training.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6004E7E9-5346-48CB-8F12-F2703157BFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCEC255-EE36-49BA-A1E5-EE27899BF773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" activeCellId="1" sqref="C3 J6"/>
+      <selection activeCell="A12" sqref="A12:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -457,6 +457,116 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{697B883F-C547-4B72-972E-FCB67DBB6DC9}"/>
@@ -464,6 +574,16 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{CB7EB58D-B9C1-4913-BB4E-87F1FCA22D29}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{675DDE76-10A4-428C-978E-864A42C1630A}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{DA4F394F-7B6B-4A5D-8F30-824CA014A9A5}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{1D0AD40F-DE36-4435-AEC2-03199D7F8EF2}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{E75B9782-A263-4F77-8A02-9481334E9C45}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{92B49A7C-F190-475C-8254-2530CF777D1E}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{5F1FC2D0-694C-4C0D-8143-51B81FE98F99}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{E7AACD7B-A0FA-4C9A-B8F6-141A1A660030}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{3498ACEF-3EC6-4B14-99BE-051F153CBE50}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{B74FEDF7-6D71-416A-A6B7-F8A5B93A8B28}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{084BC709-0E18-4E5E-8655-F871BEB47770}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{620AFAEC-CDAE-4553-9CDA-A10F6DE65658}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{50EB7B85-A9B9-4EDD-BA5E-8573D296A2F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hoàn thiện giao diện ban đào tạo, sửa model training
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/training.xlsx
+++ b/Hethongquanlylab/wwwroot/data/training.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FCE22C-33AE-4705-B2CB-E5267F0FA175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCBB0D8-4FF5-4ED6-B707-CB96277445BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="1110" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -55,13 +55,52 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/Snn0-Im3kUc</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>PT Lập trình</t>
+  </si>
+  <si>
+    <t>PT PTBT</t>
+  </si>
+  <si>
+    <t>18/08/2022</t>
+  </si>
+  <si>
+    <t>18/08/2023</t>
+  </si>
+  <si>
+    <t>18/08/2024</t>
+  </si>
+  <si>
+    <t>18/08/2025</t>
+  </si>
+  <si>
+    <t>18/08/2026</t>
+  </si>
+  <si>
+    <t>18/08/2027</t>
+  </si>
+  <si>
+    <t>18/08/2028</t>
+  </si>
+  <si>
+    <t>18/08/2029</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +112,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,9 +144,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,15 +430,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,8 +452,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -412,8 +469,14 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -423,8 +486,14 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -434,8 +503,14 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -445,8 +520,14 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -456,8 +537,14 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -467,8 +554,14 @@
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -478,8 +571,14 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -489,85 +588,46 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{697B883F-C547-4B72-972E-FCB67DBB6DC9}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{2874A540-B56E-411A-B854-6B43AE12C9BC}"/>
@@ -577,14 +637,8 @@
     <hyperlink ref="C7" r:id="rId6" xr:uid="{E53FAEA8-C4B7-4B66-B58D-70B0CA3B13DD}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{53DC2655-8FD6-49D3-855C-4725AE9894FD}"/>
     <hyperlink ref="C9" r:id="rId8" xr:uid="{762CBA57-04CB-4E63-A0A4-3711823EAFE8}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{7906CC10-542F-4115-AA10-B6649F2BB047}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{61CA7BD3-97E4-4962-9EEB-2F1CD54909BB}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{63379932-4562-4BCB-A7DF-3F13C5E95E5E}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{180D4822-EC72-4E0A-B78D-81B4ABFD02EA}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{05BD2DFC-15AF-4F88-B602-126E09252945}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{C20F3460-6E44-4267-B257-08DF7A8158AA}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{A63A3011-A48E-42C6-BA8E-F860B29610B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sửa model Member + Procedure
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/training.xlsx
+++ b/Hethongquanlylab/wwwroot/data/training.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84946D7E-7EAE-4053-AAF0-271A689D8967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB60FB5-F5D6-4B9C-BD59-A899E6865771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>kdjfdjh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">àhajd </t>
+  </si>
+  <si>
+    <t>fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdasfjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdasfjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdasfjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas fjadshfjdas</t>
   </si>
 </sst>
 </file>
@@ -171,11 +177,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,21 +466,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="75.9296875" customWidth="1"/>
+    <col min="8" max="8" width="14.86328125" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -508,10 +518,10 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -527,11 +537,11 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -551,7 +561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -571,7 +581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -591,7 +601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -611,7 +621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
@@ -631,7 +641,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -651,44 +661,333 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D17" s="2"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
       <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -701,8 +1000,24 @@
     <hyperlink ref="C7" r:id="rId6" xr:uid="{E53FAEA8-C4B7-4B66-B58D-70B0CA3B13DD}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{53DC2655-8FD6-49D3-855C-4725AE9894FD}"/>
     <hyperlink ref="C9" r:id="rId8" xr:uid="{762CBA57-04CB-4E63-A0A4-3711823EAFE8}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{34DA3A32-1921-4777-B737-477A8AFA16DC}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{CF5793A5-40D9-4489-9553-201B6EB407C7}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{E192D9DB-79C1-4C6E-BCA8-D661B19E8E80}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{F08B2F95-C30D-4163-95BF-3C4CB85E5A9D}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{5053CAEF-7383-4ECD-B616-A34B06420E24}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{90176932-AFAA-474E-9D07-5155586014F9}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{F02AB07E-D912-43CF-B6D5-C1E06A0FD13F}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{7C67B43C-89C3-40FE-B8F4-EF99F784ECF6}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{79EF15FD-DCD4-4512-8E90-DBB192303719}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{0C7AE151-F05C-49C4-B5A2-15C3D6770387}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{435A0FEF-60FA-4F06-86C3-EAF160640107}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{5CB42CB7-4209-4CF6-A76C-C70445D87583}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{8B9D0CFE-3ABC-4CD2-9587-B5500C7EECE5}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{5D1514E6-A694-46EC-BC58-88F2AED4768A}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{116F86E1-9C68-4FBB-B56F-DA1ECA88AE0C}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{B47F35D9-DACE-43EA-9F21-0E669F3FE110}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>